<commit_message>
out of range 수정
</commit_message>
<xml_diff>
--- a/ALL_class.xlsx
+++ b/ALL_class.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,27 +469,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>과학</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>영어</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>국어1</t>
+          <t>사회</t>
         </is>
       </c>
     </row>
@@ -504,12 +504,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>영어</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -519,7 +519,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>수학1</t>
         </is>
       </c>
     </row>
@@ -529,27 +529,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>국어1</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>국어1</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>국어1</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>국어1</t>
         </is>
       </c>
     </row>
@@ -559,27 +559,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>과학</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>영어</t>
+          <t>체육</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>사회</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -609,97 +609,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>수학1</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>국어1</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>수학1</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>국어2</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>수학1</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>과학</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>국어2</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>사회</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>사회</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>수학2</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>사회</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>수학1</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>국어2</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>과학</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>과학</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>수학2</t>
+          <t>영어</t>
         </is>
       </c>
     </row>
@@ -714,7 +624,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -755,7 +665,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>수학1</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -765,17 +675,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>사회</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>체육</t>
         </is>
       </c>
     </row>
@@ -785,27 +695,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>국어1</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>사회</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>과학</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>국어1</t>
         </is>
       </c>
     </row>
@@ -815,12 +725,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -830,12 +740,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>과학</t>
+          <t>사회</t>
         </is>
       </c>
     </row>
@@ -845,27 +755,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>국어1</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>수학1</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>사회</t>
+          <t>영어</t>
         </is>
       </c>
     </row>
@@ -875,117 +785,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>과학</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>영어</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>영어</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>체육</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>수학2</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>국어2</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>영어</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>국어1</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>수학1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>사회</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>체육</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>국어1</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>과학</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>영어</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>영어</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>과학</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>사회</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>수학1</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>국어1</t>
+          <t>수학1</t>
         </is>
       </c>
     </row>
@@ -1000,7 +820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1041,27 +861,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>과학</t>
+          <t>영어</t>
         </is>
       </c>
     </row>
@@ -1071,22 +891,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>과학</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>사회</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1106,22 +926,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>사회</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>과학</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>체육</t>
         </is>
       </c>
     </row>
@@ -1131,22 +951,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>국어1</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>영어</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>수학1</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1161,117 +981,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>수학1</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>국어1</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>국어1</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>사회</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>국어1</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>과학</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>사회</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>영어</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>영어</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>국어2</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>영어</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>영어</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>수학2</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>과학</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>수학2</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>수학1</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>국어1</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>체육</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1016,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1327,7 +1057,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>과학</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1337,17 +1067,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>과학</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>수학1</t>
         </is>
       </c>
     </row>
@@ -1357,27 +1087,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>수학1</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>사회</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>영어</t>
+          <t>체육</t>
         </is>
       </c>
     </row>
@@ -1387,27 +1117,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>사회</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>수학1</t>
+          <t>영어</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>수학1</t>
+          <t>영어</t>
         </is>
       </c>
     </row>
@@ -1422,22 +1152,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>수학1</t>
+          <t>국어1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>국어1</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>수학2</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>체육</t>
+          <t>국어1</t>
         </is>
       </c>
     </row>
@@ -1447,17 +1177,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>국어1</t>
+          <t>체육</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>과학</t>
+          <t>수학1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>국어2</t>
+          <t>사회</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1467,97 +1197,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>과학</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>영어</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>체육</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>수학1</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>영어</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>사회</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>체육</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>국어1</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>과학</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>국어1</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>국어1</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>국어2</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>사회</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>영어</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>국어2</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>국어2</t>
+          <t>사회</t>
         </is>
       </c>
     </row>

</xml_diff>